<commit_message>
9/1/2019 created iniital SQL files
</commit_message>
<xml_diff>
--- a/docs/20190828 ProjectNotes.xlsx
+++ b/docs/20190828 ProjectNotes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asia8_000\Desktop\z.Temp\Rice_Data_Analytics_Boot_Camp\005 - 13-ETL-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asia8_000\Desktop\z.Temp\Rice_Data_Analytics_Boot_Camp\005 - 13-ETL-Project\Project_ETL\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070A6293-C47E-4FB6-BF19-8647F05E6380}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89024AEB-5FE9-42AC-B0D3-26AB50F55348}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A67F39CA-D464-4BAC-9DD4-5E934DEE64C7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>20190828 Class Notes</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Folder structure</t>
   </si>
   <si>
-    <t>Daniel will create github repo, add</t>
-  </si>
-  <si>
     <t>create folder structure</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>Responsible Party</t>
   </si>
   <si>
-    <t>Neuroscience Research Compensation</t>
-  </si>
-  <si>
     <t>Are Neuroscience Professors being adequately compensated by their academic output?</t>
   </si>
   <si>
@@ -274,7 +268,40 @@
     <t>compensated proportionately to academic output</t>
   </si>
   <si>
-    <t>*Add to slack</t>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Daniel will create github repo, and</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Neuroscience Research </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Compensation</t>
+    </r>
+  </si>
+  <si>
+    <t>http://apps.who.int/gho/data/node.main.MHPOLFIN?lang=en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mental health governance
+Data by country </t>
   </si>
 </sst>
 </file>
@@ -283,9 +310,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +409,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +438,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,7 +479,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -432,12 +489,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1110,197 +1184,274 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE14A64-3AF6-4484-BD3F-3CA820D7F95C}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.77734375" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G1" s="9">
         <v>745</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G2" s="9">
         <v>1573</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="G3" s="9">
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G4" s="10">
         <f>SUM(G1:G3)</f>
         <v>2733</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>52</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>53</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K15" t="s">
         <v>54</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="N16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>43705</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>43708</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>43715</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="K24" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="16">
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="23"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="16">
+        <v>43706</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="K19" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F21" t="s">
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="J31" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="F32" t="s">
+        <v>71</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8">
-        <v>43705</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="8">
-        <v>43708</v>
-      </c>
-      <c r="B33" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="8">
-        <v>43715</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A11" r:id="rId1" xr:uid="{C109E03A-F268-4E03-A4E9-5B13DEAA5551}"/>
     <hyperlink ref="A12" r:id="rId2" xr:uid="{FD75C7BF-A17C-4BFA-AECC-98DD3BD15849}"/>
+    <hyperlink ref="A13" r:id="rId3" xr:uid="{79BCAD6C-A9B6-40E9-A7BF-358CD714CBD2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added link to new data, and updated my responsibilities in the project notes
</commit_message>
<xml_diff>
--- a/docs/20190828 ProjectNotes.xlsx
+++ b/docs/20190828 ProjectNotes.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asia8_000\Desktop\z.Temp\Rice_Data_Analytics_Boot_Camp\005 - 13-ETL-Project\Project_ETL\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamcopeland/Desktop/Project_ETL/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89024AEB-5FE9-42AC-B0D3-26AB50F55348}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC08A795-EAE3-8949-ADEE-5EBDEF2BBD50}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A67F39CA-D464-4BAC-9DD4-5E934DEE64C7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28860" windowHeight="16000" activeTab="1" xr2:uid="{A67F39CA-D464-4BAC-9DD4-5E934DEE64C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Project" sheetId="2" r:id="rId2"/>
     <sheet name="MarkdownExample" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>20190828 Class Notes</t>
   </si>
@@ -302,6 +303,15 @@
   <si>
     <t xml:space="preserve">Mental health governance
 Data by country </t>
+  </si>
+  <si>
+    <t>Finding data</t>
+  </si>
+  <si>
+    <t>Data cleaning</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -927,92 +937,92 @@
       <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1020,57 +1030,57 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>28</v>
       </c>
@@ -1078,27 +1088,27 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>33</v>
       </c>
@@ -1106,72 +1116,72 @@
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>48</v>
       </c>
@@ -1184,64 +1194,64 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE14A64-3AF6-4484-BD3F-3CA820D7F95C}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.77734375" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="18" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G1" s="9">
         <v>745</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G2" s="9">
         <v>1573</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G3" s="9">
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G4" s="10">
         <f>SUM(G1:G3)</f>
         <v>2733</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>83</v>
       </c>
@@ -1249,7 +1259,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
@@ -1266,7 +1276,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>55</v>
       </c>
@@ -1277,12 +1287,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>76</v>
       </c>
@@ -1290,7 +1300,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>43705</v>
       </c>
@@ -1298,7 +1308,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>43708</v>
       </c>
@@ -1306,7 +1316,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>43715</v>
       </c>
@@ -1314,10 +1324,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>73</v>
       </c>
@@ -1339,7 +1349,7 @@
       </c>
       <c r="L24" s="14"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="22" t="s">
         <v>58</v>
       </c>
@@ -1358,7 +1368,7 @@
         <v>43705</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
@@ -1375,10 +1385,10 @@
         <v>43706</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>61</v>
       </c>
@@ -1392,57 +1402,79 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" t="s">
-        <v>62</v>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="G29" t="s">
+        <v>85</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="G30" t="s">
+        <v>86</v>
       </c>
       <c r="J30" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="F31" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" t="s">
+        <v>62</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="F34" t="s">
         <v>70</v>
       </c>
-      <c r="J31" s="20" t="s">
+      <c r="J34" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="F32" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="F35" t="s">
         <v>71</v>
       </c>
-      <c r="J32" s="20" t="s">
+      <c r="J35" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F37" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1463,7 +1495,7 @@
       <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>